<commit_message>
Updated Blog and weekly timekeeping spreadsheet
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\blogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7DA82-F436-4D64-B195-D91D0EF58885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200FEB12-29D4-4EB0-8EF2-8224EFAFAD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
+    <workbookView xWindow="32310" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
   <si>
     <t>Week 1</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Junit</t>
+  </si>
+  <si>
+    <t>Week 5</t>
   </si>
 </sst>
 </file>
@@ -279,6 +282,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -302,6 +310,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -325,6 +338,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -348,6 +366,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -371,6 +394,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -394,6 +422,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -419,6 +452,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -444,6 +482,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-D1BE-4586-AFC2-13602B84976F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -537,28 +580,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1606,7 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1571,8 +1614,9 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1586,8 +1630,11 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1603,8 +1650,11 @@
       <c r="E3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1621,7 +1671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1637,8 +1687,11 @@
       <c r="E5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1648,8 +1701,14 @@
       <c r="C6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1665,8 +1724,11 @@
       <c r="E7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1682,8 +1744,11 @@
       <c r="E8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1699,8 +1764,11 @@
       <c r="E9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1716,8 +1784,11 @@
       <c r="E10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1731,50 +1802,71 @@
       </c>
       <c r="D11">
         <f>SUM(D3:D10)</f>
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E11">
         <f>SUM(E3:E10)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F3:F10)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <f>SUM(B3:J3)</f>
-        <v>31</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1782,170 +1874,162 @@
         <f>SUM(B4:J4)</f>
         <v>19</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="L15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>12</v>
+      </c>
+      <c r="P15">
         <v>8</v>
       </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>4</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B16">
         <f>SUM(B5:J5)</f>
-        <v>33</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16">
+        <v>38</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>3</v>
       </c>
-      <c r="H16">
+      <c r="P16">
         <v>4</v>
       </c>
-      <c r="I16">
-        <v>12</v>
-      </c>
-      <c r="J16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17">
         <f>SUM(B6:J6)</f>
-        <v>15</v>
-      </c>
-      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17">
+        <f>SUM(M14:M16)</f>
         <v>6</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <f>SUM(N14:N16)</f>
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <f>SUM(O14:O16)</f>
+        <v>19</v>
+      </c>
+      <c r="P17">
+        <f>SUM(P14:P16)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <f>SUM(B7:I7)</f>
-        <v>29</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18">
-        <f>SUM(G15:G17)</f>
-        <v>6</v>
-      </c>
-      <c r="H18">
-        <f>SUM(H15:H17)</f>
-        <v>6</v>
-      </c>
-      <c r="I18">
-        <f>SUM(I15:I17)</f>
-        <v>19</v>
-      </c>
-      <c r="J18">
-        <f>SUM(J15:J17)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19">
         <f>SUM(B8:I8)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20">
         <f>SUM(B9:J9)</f>
-        <v>38</v>
-      </c>
-      <c r="G20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21">
         <f>SUM(B10:J10)</f>
-        <v>45</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>237</v>
-      </c>
-      <c r="G22" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H22">
+      <c r="M22">
         <v>2</v>
       </c>
-      <c r="I22">
+      <c r="N22">
         <v>7</v>
       </c>
-      <c r="J22">
+      <c r="O22">
         <v>11</v>
       </c>
-      <c r="K22">
+      <c r="P22">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1953,8 +2037,9 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -1968,8 +2053,11 @@
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1985,15 +2073,19 @@
       <c r="E27">
         <v>6</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2009,21 +2101,27 @@
       <c r="E28">
         <v>6</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q28" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -2043,61 +2141,70 @@
         <f>SUM(E27:E28)</f>
         <v>12</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <v>5</v>
       </c>
-      <c r="J29">
+      <c r="O29">
         <v>5</v>
       </c>
-      <c r="K29">
+      <c r="P29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="2" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H30">
+      <c r="M30">
         <v>4</v>
       </c>
-      <c r="I30">
+      <c r="N30">
         <v>4</v>
       </c>
-      <c r="J30">
+      <c r="O30">
         <v>5</v>
       </c>
-      <c r="K30">
+      <c r="P30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G31" t="s">
+      <c r="Q30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
         <v>21</v>
       </c>
-      <c r="H31">
-        <f>SUM(H29:H30)</f>
+      <c r="M31">
+        <f>SUM(M29:M30)</f>
         <v>4</v>
       </c>
-      <c r="I31">
-        <f>SUM(I29:I30)</f>
+      <c r="N31">
+        <f>SUM(N29:N30)</f>
         <v>9</v>
       </c>
-      <c r="J31">
-        <f>SUM(J29:J30)</f>
+      <c r="O31">
+        <f>SUM(O29:O30)</f>
         <v>10</v>
       </c>
-      <c r="K31">
-        <f>SUM(K29:K30)</f>
+      <c r="P31">
+        <f>SUM(P29:P30)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2105,8 +2212,9 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2120,8 +2228,11 @@
       <c r="E34" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2137,15 +2248,19 @@
       <c r="E35">
         <v>2</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2161,21 +2276,27 @@
       <c r="E36">
         <v>2</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1" t="s">
+      <c r="F36">
         <v>1</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="L36" s="1"/>
+      <c r="M36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q36" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2191,23 +2312,29 @@
       <c r="E37">
         <v>6</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="F37">
         <v>5</v>
       </c>
-      <c r="H37">
+      <c r="L37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M37">
         <v>2</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -2219,65 +2346,78 @@
         <f>SUM(E35:E37)</f>
         <v>10</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="F38">
         <v>9</v>
       </c>
-      <c r="H38">
+      <c r="L38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M38">
         <v>5</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G39" s="2" t="s">
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H39">
+      <c r="M39">
         <v>4</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G40" t="s">
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
         <v>21</v>
       </c>
-      <c r="H40">
-        <f>SUM(H37:H39)</f>
+      <c r="M40">
+        <f>SUM(M37:M39)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <f>SUM(Q37:Q39)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42">
-        <f>SUM(G18:J18)</f>
+        <f>SUM(M17:P17)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2286,34 +2426,34 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
       <c r="B44">
-        <f>SUM(H40:K40)</f>
+        <f>SUM(M40:P40)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(H31:K31)</f>
+        <f>SUM(M31:P31)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(H22:K22)</f>
+        <f>SUM(M22:P22)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Updated Time sheet to include those pesky missing blogs from yesterday <3
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200FEB12-29D4-4EB0-8EF2-8224EFAFAD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F589B-7070-46E7-9BBC-B33C179252CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32310" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t>Week 1</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Week 5</t>
+  </si>
+  <si>
+    <t>Tyw</t>
+  </si>
+  <si>
+    <t>Tyw1</t>
   </si>
 </sst>
 </file>
@@ -583,13 +589,13 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37</c:v>
@@ -1261,16 +1267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1595,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1612,7 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1616,7 +1622,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1634,7 +1640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1670,8 +1676,11 @@
       <c r="E4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1691,7 +1700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1707,8 +1716,11 @@
       <c r="E6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1728,7 +1740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1748,7 +1760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1768,7 +1780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1810,39 +1822,17 @@
       </c>
       <c r="F11">
         <f>SUM(F3:F10)</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1850,47 +1840,17 @@
         <f>SUM(B3:J3)</f>
         <v>39</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14">
-        <v>3</v>
-      </c>
-      <c r="N14">
-        <v>2</v>
-      </c>
-      <c r="O14">
-        <v>4</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <f>SUM(B4:J4)</f>
-        <v>19</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15">
-        <v>3</v>
-      </c>
-      <c r="N15">
-        <v>4</v>
-      </c>
-      <c r="O15">
-        <v>12</v>
-      </c>
-      <c r="P15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1898,51 +1858,17 @@
         <f>SUM(B5:J5)</f>
         <v>38</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>3</v>
-      </c>
-      <c r="P16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17">
         <f>SUM(B6:J6)</f>
-        <v>30</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17">
-        <f>SUM(M14:M16)</f>
-        <v>6</v>
-      </c>
-      <c r="N17">
-        <f>SUM(N14:N16)</f>
-        <v>6</v>
-      </c>
-      <c r="O17">
-        <f>SUM(O14:O16)</f>
-        <v>19</v>
-      </c>
-      <c r="P17">
-        <f>SUM(P14:P16)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1960,7 +1886,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1968,16 +1894,8 @@
         <f>SUM(B9:J9)</f>
         <v>54</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1985,51 +1903,41 @@
         <f>SUM(B10:J10)</f>
         <v>53</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>305</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M22">
-        <v>2</v>
-      </c>
-      <c r="N22">
-        <v>7</v>
-      </c>
-      <c r="O22">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P22">
-        <v>8</v>
-      </c>
-      <c r="Q22">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2038,8 +1946,23 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2056,8 +1979,23 @@
       <c r="F26" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>12</v>
+      </c>
+      <c r="L26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2076,16 +2014,23 @@
       <c r="F27">
         <v>4</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2104,107 +2049,117 @@
       <c r="F28">
         <v>3</v>
       </c>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1" t="s">
+      <c r="H28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28">
+        <f>SUM(I25:I27)</f>
+        <v>6</v>
+      </c>
+      <c r="J28">
+        <f>SUM(J25:J27)</f>
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <f>SUM(K25:K27)</f>
+        <v>19</v>
+      </c>
+      <c r="L28">
+        <f>SUM(L25:L27)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <f>SUM(B27:B29)</f>
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <f>SUM(C27:C29)</f>
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D27:D29)</f>
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <f>SUM(E27:E29)</f>
+        <v>12</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29">
-        <f>SUM(B27:B28)</f>
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <f>SUM(C27:C28)</f>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>7</v>
+      </c>
+      <c r="K32">
         <v>11</v>
       </c>
-      <c r="D29">
-        <f>SUM(D27:D28)</f>
-        <v>9</v>
-      </c>
-      <c r="E29">
-        <f>SUM(E27:E28)</f>
-        <v>12</v>
-      </c>
-      <c r="F29">
-        <v>7</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>5</v>
-      </c>
-      <c r="O29">
-        <v>5</v>
-      </c>
-      <c r="P29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M30">
-        <v>4</v>
-      </c>
-      <c r="N30">
-        <v>4</v>
-      </c>
-      <c r="O30">
-        <v>5</v>
-      </c>
-      <c r="P30">
+      <c r="L32">
         <v>8</v>
       </c>
-      <c r="Q30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L31" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31">
-        <f>SUM(M29:M30)</f>
-        <v>4</v>
-      </c>
-      <c r="N31">
-        <f>SUM(N29:N30)</f>
-        <v>9</v>
-      </c>
-      <c r="O31">
-        <f>SUM(O29:O30)</f>
-        <v>10</v>
-      </c>
-      <c r="P31">
-        <f>SUM(P29:P30)</f>
-        <v>12</v>
-      </c>
-      <c r="Q31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2214,7 +2169,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2231,8 +2186,16 @@
       <c r="F34" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2251,16 +2214,24 @@
       <c r="F35">
         <v>3</v>
       </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2279,24 +2250,26 @@
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>5</v>
+      </c>
+      <c r="L36">
+        <v>4</v>
+      </c>
+      <c r="M36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2315,26 +2288,26 @@
       <c r="F37">
         <v>5</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <v>8</v>
       </c>
       <c r="M37">
         <v>2</v>
       </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -2349,117 +2322,195 @@
       <c r="F38">
         <v>9</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="H38" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38">
+        <f>SUM(I36:I37)</f>
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <f>SUM(J36:J37)</f>
         <v>9</v>
       </c>
+      <c r="K38">
+        <f>SUM(K36:K37)</f>
+        <v>10</v>
+      </c>
+      <c r="L38">
+        <f>SUM(L36:L37)</f>
+        <v>12</v>
+      </c>
       <c r="M38">
-        <v>5</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M39">
-        <v>4</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L40" t="s">
-        <v>21</v>
-      </c>
-      <c r="M40">
-        <f>SUM(M37:M39)</f>
-        <v>11</v>
-      </c>
-      <c r="Q40">
-        <f>SUM(Q37:Q39)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42">
-        <f>SUM(M17:P17)</f>
+        <f>SUM(I28:L28)</f>
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43">
-        <f>SUM(B29:E29)</f>
+        <f>SUM(B30:E30)</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
       <c r="B44">
-        <f>SUM(M40:P40)</f>
+        <f>SUM(F47:I47)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(M31:P31)</f>
+        <f>SUM(I38:L38)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(M22:P22)</f>
+        <f>SUM(I32:L32)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E46" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
       <c r="B47">
         <f>SUM(B38:E38)</f>
         <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47">
+        <f>SUM(F43:F46)</f>
+        <v>11</v>
+      </c>
+      <c r="J47">
+        <f>SUM(J43:J46)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated blogs and timekeeping speadsheet		:
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F589B-7070-46E7-9BBC-B33C179252CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92C73B7-0F5B-40FB-B125-761538C775CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32310" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
+    <workbookView xWindow="3510" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
   <si>
     <t>Week 1</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Tyw1</t>
+  </si>
+  <si>
+    <t>Week 6</t>
   </si>
 </sst>
 </file>
@@ -185,10 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,28 +590,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,16 +1271,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1601,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,7 +1616,7 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1621,8 +1625,9 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1639,8 +1644,11 @@
       <c r="F2" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1659,8 +1667,11 @@
       <c r="F3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1680,7 +1691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1697,10 +1708,13 @@
         <v>11</v>
       </c>
       <c r="F5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1719,8 +1733,11 @@
       <c r="F6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1739,8 +1756,11 @@
       <c r="F7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1759,8 +1779,11 @@
       <c r="F8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1779,8 +1802,11 @@
       <c r="F9">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1799,8 +1825,11 @@
       <c r="F10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1822,26 +1851,30 @@
       </c>
       <c r="F11">
         <f>SUM(F3:F10)</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="G11">
+        <f>SUM(G3:G10)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <f>SUM(B3:J3)</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1850,94 +1883,124 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B16">
         <f>SUM(B5:J5)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17">
         <f>SUM(B6:J6)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <f>SUM(B7:I7)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19">
         <f>SUM(B8:I8)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20">
         <f>SUM(B9:J9)</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21">
         <f>SUM(B10:J10)</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H24" s="1"/>
-      <c r="I24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>12</v>
+      </c>
+      <c r="M24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1946,23 +2009,24 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="H25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25">
+      <c r="G25" s="3"/>
+      <c r="I25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>3</v>
       </c>
-      <c r="J25">
-        <v>2</v>
-      </c>
-      <c r="K25">
+      <c r="M25">
         <v>4</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -1979,23 +2043,28 @@
       <c r="F26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26">
-        <v>3</v>
+      <c r="G26" s="3"/>
+      <c r="I26" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <f>SUM(J23:J25)</f>
+        <v>6</v>
       </c>
       <c r="K26">
+        <f>SUM(K23:K25)</f>
+        <v>6</v>
+      </c>
+      <c r="L26">
+        <f>SUM(L23:L25)</f>
+        <v>19</v>
+      </c>
+      <c r="M26">
+        <f>SUM(M23:M25)</f>
         <v>12</v>
       </c>
-      <c r="L26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2014,23 +2083,8 @@
       <c r="F27">
         <v>4</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-      <c r="L27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2049,27 +2103,17 @@
       <c r="F28">
         <v>3</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28">
-        <f>SUM(I25:I27)</f>
-        <v>6</v>
-      </c>
-      <c r="J28">
-        <f>SUM(J25:J27)</f>
-        <v>6</v>
-      </c>
-      <c r="K28">
-        <f>SUM(K25:K27)</f>
-        <v>19</v>
-      </c>
-      <c r="L28">
-        <f>SUM(L25:L27)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2088,9 +2132,28 @@
       <c r="F29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B30">
@@ -2112,54 +2175,81 @@
       <c r="F30">
         <v>7</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H31" s="1"/>
-      <c r="I31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K31" s="1" t="s">
+      <c r="I30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>7</v>
+      </c>
+      <c r="L30">
         <v>11</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32">
+      <c r="M30">
+        <v>8</v>
+      </c>
+      <c r="N30">
+        <v>13</v>
+      </c>
+      <c r="O30">
         <v>2</v>
       </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J32">
+        <f>SUM(J30:J31)</f>
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <f>SUM(K30:K31)</f>
         <v>7</v>
       </c>
-      <c r="K32">
+      <c r="L32">
+        <f>SUM(L30:L31)</f>
         <v>11</v>
       </c>
-      <c r="L32">
+      <c r="M32">
+        <f>SUM(M30:M31)</f>
         <v>8</v>
       </c>
-      <c r="M32">
+      <c r="N32">
+        <f>SUM(N30:N31)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <f>SUM(O30:O31)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2168,8 +2258,9 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2186,16 +2277,20 @@
       <c r="F34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2214,24 +2309,30 @@
       <c r="F35">
         <v>3</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2250,26 +2351,32 @@
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
       <c r="J36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>5</v>
       </c>
       <c r="L36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2288,28 +2395,42 @@
       <c r="F37">
         <v>5</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="G37">
         <v>5</v>
       </c>
-      <c r="I37">
-        <v>4</v>
+      <c r="I37" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="J37">
         <v>4</v>
       </c>
       <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
         <v>5</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>8</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="O37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="B38">
+        <f>SUM(B35:B37)</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>SUM(C35:C37)</f>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>SUM(D35:D37)</f>
@@ -2322,30 +2443,38 @@
       <c r="F38">
         <v>9</v>
       </c>
-      <c r="H38" t="s">
+      <c r="G38">
+        <f>SUM(G35:G37)</f>
+        <v>16</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="I38">
-        <f>SUM(I36:I37)</f>
-        <v>4</v>
       </c>
       <c r="J38">
         <f>SUM(J36:J37)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K38">
         <f>SUM(K36:K37)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L38">
         <f>SUM(L36:L37)</f>
+        <v>10</v>
+      </c>
+      <c r="M38">
+        <f>SUM(M36:M37)</f>
         <v>12</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <f>SUM(O36:O37)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2359,13 +2488,14 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42">
-        <f>SUM(I28:L28)</f>
+        <f>SUM(J26:M26)</f>
         <v>43</v>
       </c>
       <c r="E42" s="1"/>
@@ -2384,14 +2514,17 @@
       <c r="J42" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K42" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43">
-        <f>SUM(B30:E30)</f>
-        <v>37</v>
+        <f>SUM(B30:F30)</f>
+        <v>44</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>5</v>
@@ -2411,14 +2544,17 @@
       <c r="J43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
       <c r="B44">
-        <f>SUM(F47:I47)</f>
-        <v>11</v>
+        <f>SUM(F47:K47)</f>
+        <v>24</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>9</v>
@@ -2438,14 +2574,17 @@
       <c r="J44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(I38:L38)</f>
-        <v>35</v>
+        <f>SUM(J38:O38)</f>
+        <v>45</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>6</v>
@@ -2465,14 +2604,17 @@
       <c r="J45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(I32:L32)</f>
-        <v>28</v>
+        <f>SUM(J32:O32)</f>
+        <v>49</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>31</v>
@@ -2492,25 +2634,44 @@
       <c r="J46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
       <c r="B47">
-        <f>SUM(B38:E38)</f>
-        <v>11</v>
-      </c>
-      <c r="E47" t="s">
+        <f>SUM(B38:G38)</f>
+        <v>36</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F47">
         <f>SUM(F43:F46)</f>
         <v>11</v>
       </c>
+      <c r="G47">
+        <f>SUM(G43:G46)</f>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <f>SUM(H43:H46)</f>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f>SUM(I43:I46)</f>
+        <v>0</v>
+      </c>
       <c r="J47">
         <f>SUM(J43:J46)</f>
         <v>5</v>
+      </c>
+      <c r="K47">
+        <f>SUM(K43:K46)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added blog, updated spreadsheet. See spreadsheet for rough timeline of goals
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92C73B7-0F5B-40FB-B125-761538C775CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653D0075-AEAC-406C-BB8B-3BD60B134467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>Week 1</t>
   </si>
@@ -135,6 +135,57 @@
   </si>
   <si>
     <t>Week 6</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Front-end and Backend finished and ready for docking</t>
+  </si>
+  <si>
+    <t>Back and front need to be at least partially integrated</t>
+  </si>
+  <si>
+    <t>Junit package 90% done</t>
+  </si>
+  <si>
+    <t>Design Specification feedback resolved</t>
+  </si>
+  <si>
+    <t>There needs to be partial implementation reviewed  and submitted to src</t>
+  </si>
+  <si>
+    <t>Shit hits the fan</t>
+  </si>
+  <si>
+    <t>Celebratory drink(or cry)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code must be submitted </t>
+  </si>
+  <si>
+    <t>Maintenance manual needs to be made</t>
+  </si>
+  <si>
+    <t>Any additions to documentation have to be done starting this week</t>
+  </si>
+  <si>
+    <t>Acceptance tests  with client will begin sometime over the next 3 days</t>
+  </si>
+  <si>
+    <t>Final submission of documents</t>
+  </si>
+  <si>
+    <t>Second celebratory drink(or sob)</t>
+  </si>
+  <si>
+    <t>Week 7</t>
   </si>
 </sst>
 </file>
@@ -156,7 +207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +226,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,11 +245,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,28 +648,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>45</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>45</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>59</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,16 +1329,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1597,7 +1655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1605,18 +1663,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1626,8 +1685,9 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1647,8 +1707,16 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1670,8 +1738,14 @@
       <c r="G3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1690,8 +1764,14 @@
       <c r="F4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1713,8 +1793,17 @@
       <c r="G5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>45032</v>
+      </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1736,8 +1825,17 @@
       <c r="G6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>45039</v>
+      </c>
+      <c r="R6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1759,8 +1857,17 @@
       <c r="G7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>45039</v>
+      </c>
+      <c r="R7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1782,8 +1889,17 @@
       <c r="G8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>45039</v>
+      </c>
+      <c r="R8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1805,8 +1921,17 @@
       <c r="G9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>45044</v>
+      </c>
+      <c r="R9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1828,53 +1953,92 @@
       <c r="G10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>45048</v>
+      </c>
+      <c r="R10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B11">
-        <f>SUM(B3:B10)</f>
+        <f t="shared" ref="B11:G11" si="0">SUM(B3:B10)</f>
         <v>52</v>
       </c>
       <c r="C11">
-        <f>SUM(C3:C10)</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="D11">
-        <f>SUM(D3:D10)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="E11">
-        <f>SUM(E3:E10)</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="F11">
-        <f>SUM(F3:F10)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="G11">
-        <f>SUM(G3:G10)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f>SUM(H3:H10)</f>
+        <v>65</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>45051</v>
+      </c>
+      <c r="R11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q12" s="4">
+        <v>45051</v>
+      </c>
+      <c r="R12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q13" s="4">
+        <v>45053</v>
+      </c>
+      <c r="R13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <f>SUM(B3:J3)</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>45053</v>
+      </c>
+      <c r="R14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1882,125 +2046,143 @@
         <f>SUM(B4:J4)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q15" s="4">
+        <v>45055</v>
+      </c>
+      <c r="R15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B16">
         <f>SUM(B5:J5)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>45058</v>
+      </c>
+      <c r="R16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17">
         <f>SUM(B6:J6)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>45058</v>
+      </c>
+      <c r="R17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <f>SUM(B7:I7)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19">
         <f>SUM(B8:I8)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20">
         <f>SUM(B9:J9)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21">
         <f>SUM(B10:J10)</f>
-        <v>59</v>
-      </c>
-      <c r="I21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>377</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I23" s="2" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J23">
+      <c r="M23">
         <v>3</v>
       </c>
-      <c r="K23">
+      <c r="N23">
         <v>2</v>
       </c>
-      <c r="L23">
+      <c r="O23">
         <v>4</v>
       </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I24" s="2" t="s">
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J24">
+      <c r="M24">
         <v>3</v>
       </c>
-      <c r="K24">
+      <c r="N24">
         <v>4</v>
       </c>
-      <c r="L24">
+      <c r="O24">
         <v>12</v>
       </c>
-      <c r="M24">
+      <c r="P24">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2009,24 +2191,23 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
         <v>3</v>
       </c>
-      <c r="M25">
+      <c r="P25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2043,28 +2224,30 @@
       <c r="F26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="I26" s="2" t="s">
+      <c r="G26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="J26">
-        <f>SUM(J23:J25)</f>
-        <v>6</v>
-      </c>
-      <c r="K26">
-        <f>SUM(K23:K25)</f>
-        <v>6</v>
-      </c>
-      <c r="L26">
-        <f>SUM(L23:L25)</f>
-        <v>19</v>
       </c>
       <c r="M26">
         <f>SUM(M23:M25)</f>
+        <v>6</v>
+      </c>
+      <c r="N26">
+        <f>SUM(N23:N25)</f>
+        <v>6</v>
+      </c>
+      <c r="O26">
+        <f>SUM(O23:O25)</f>
+        <v>19</v>
+      </c>
+      <c r="P26">
+        <f>SUM(P23:P25)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2084,7 +2267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2103,17 +2286,20 @@
       <c r="F28">
         <v>3</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2132,27 +2318,27 @@
       <c r="F29">
         <v>2</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="J29" s="1"/>
       <c r="K29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2175,35 +2361,36 @@
       <c r="F30">
         <v>7</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="G30">
+        <f>SUM(G27:G29)</f>
+        <v>1</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>2</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>7</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>11</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>8</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>13</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I31" s="2" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
       <c r="K31">
         <v>0</v>
       </c>
@@ -2217,39 +2404,42 @@
         <v>0</v>
       </c>
       <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I32" s="2" t="s">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J32">
-        <f>SUM(J30:J31)</f>
+      <c r="K32">
+        <f t="shared" ref="K32:P32" si="1">SUM(K30:K31)</f>
         <v>2</v>
       </c>
-      <c r="K32">
-        <f>SUM(K30:K31)</f>
+      <c r="L32">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L32">
-        <f>SUM(L30:L31)</f>
+      <c r="M32">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="M32">
-        <f>SUM(M30:M31)</f>
+      <c r="N32">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="N32">
-        <f>SUM(N30:N31)</f>
+      <c r="O32">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="O32">
-        <f>SUM(O30:O31)</f>
+      <c r="P32">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2260,7 +2450,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2280,17 +2470,20 @@
       <c r="G34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="H34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2312,27 +2505,30 @@
       <c r="G35">
         <v>5</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="J35" s="1"/>
       <c r="K35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2354,29 +2550,32 @@
       <c r="G36">
         <v>6</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
       <c r="K36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L36">
         <v>5</v>
       </c>
       <c r="M36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N36">
         <v>4</v>
       </c>
       <c r="O36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2398,29 +2597,32 @@
       <c r="G37">
         <v>5</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="J37">
-        <v>4</v>
       </c>
       <c r="K37">
         <v>4</v>
       </c>
       <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="M37">
         <v>5</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>8</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>2</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2447,34 +2649,38 @@
         <f>SUM(G35:G37)</f>
         <v>16</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="H38">
+        <f>SUM(H35:H37)</f>
+        <v>14</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="J38">
-        <f>SUM(J36:J37)</f>
-        <v>4</v>
       </c>
       <c r="K38">
         <f>SUM(K36:K37)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L38">
         <f>SUM(L36:L37)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M38">
         <f>SUM(M36:M37)</f>
+        <v>10</v>
+      </c>
+      <c r="N38">
+        <f>SUM(N36:N37)</f>
         <v>12</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>6</v>
       </c>
-      <c r="O38">
-        <f>SUM(O36:O37)</f>
+      <c r="P38">
+        <f>SUM(P36:P37)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2490,12 +2696,12 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42">
-        <f>SUM(J26:M26)</f>
+        <f>SUM(M26:P26)</f>
         <v>43</v>
       </c>
       <c r="E42" s="1"/>
@@ -2517,8 +2723,11 @@
       <c r="K42" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2547,8 +2756,11 @@
       <c r="K43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -2577,13 +2789,16 @@
       <c r="K44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(J38:O38)</f>
+        <f>SUM(K38:P38)</f>
         <v>45</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -2607,13 +2822,16 @@
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(J32:O32)</f>
+        <f>SUM(K32:P32)</f>
         <v>49</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -2637,8 +2855,11 @@
       <c r="K46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -2650,28 +2871,32 @@
         <v>21</v>
       </c>
       <c r="F47">
-        <f>SUM(F43:F46)</f>
+        <f t="shared" ref="F47:K47" si="2">SUM(F43:F46)</f>
         <v>11</v>
       </c>
       <c r="G47">
-        <f>SUM(G43:G46)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H47">
-        <f>SUM(H43:H46)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I47">
-        <f>SUM(I43:I46)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J47">
-        <f>SUM(J43:J46)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K47">
-        <f>SUM(K43:K46)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
+      </c>
+      <c r="L47">
+        <f>SUM(L43:L46)</f>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added  missing blogs to timesheet
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653D0075-AEAC-406C-BB8B-3BD60B134467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503E1DB2-F191-44B8-A2E6-9FA5ECD7FCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Week 1</t>
   </si>
@@ -651,7 +651,7 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>64</c:v>
@@ -1666,7 +1666,7 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,6 +1764,12 @@
       <c r="F4">
         <v>8</v>
       </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
       <c r="Q4" t="s">
         <v>35</v>
       </c>
@@ -1989,11 +1995,11 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H11">
         <f>SUM(H3:H10)</f>
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="Q11" s="4">
         <v>45051</v>
@@ -2044,7 +2050,7 @@
       </c>
       <c r="B15">
         <f>SUM(B4:J4)</f>
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="Q15" s="4">
         <v>45055</v>
@@ -2132,7 +2138,7 @@
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>442</v>
+        <v>457</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
@@ -2439,7 +2445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2450,7 +2456,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2483,7 +2489,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2527,8 +2533,11 @@
       <c r="P35" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2572,10 +2581,13 @@
         <v>4</v>
       </c>
       <c r="P36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="Q36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2621,8 +2633,11 @@
       <c r="P37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2677,10 +2692,13 @@
       </c>
       <c r="P38">
         <f>SUM(P36:P37)</f>
+        <v>7</v>
+      </c>
+      <c r="Q38">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2696,7 +2714,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2727,7 +2745,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2760,7 +2778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -2793,13 +2811,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
         <f>SUM(K38:P38)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>6</v>
@@ -2826,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -2859,7 +2877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added blog and updated timesheet.
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503E1DB2-F191-44B8-A2E6-9FA5ECD7FCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E355F4-A051-4832-9146-CDF5EB810641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
   <si>
     <t>Week 1</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
   </si>
 </sst>
 </file>
@@ -648,28 +651,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>54</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1329,16 +1332,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1663,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1678,7 @@
     <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1686,8 +1689,9 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1710,13 +1714,16 @@
       <c r="H2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="I2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1741,11 +1748,14 @@
       <c r="H3">
         <v>8</v>
       </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="I3">
+        <v>4</v>
+      </c>
       <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1770,14 +1780,14 @@
       <c r="H4">
         <v>9</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>35</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1802,14 +1812,17 @@
       <c r="H5">
         <v>13</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="S5" s="4">
         <v>45032</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1834,14 +1847,14 @@
       <c r="H6">
         <v>6</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="S6" s="4">
         <v>45039</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1866,14 +1879,17 @@
       <c r="H7">
         <v>9</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="S7" s="4">
         <v>45039</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1898,14 +1914,17 @@
       <c r="H8">
         <v>7</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="S8" s="4">
         <v>45039</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1930,14 +1949,14 @@
       <c r="H9">
         <v>12</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="S9" s="4">
         <v>45044</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1962,14 +1981,17 @@
       <c r="H10">
         <v>10</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="S10" s="4">
         <v>45048</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2001,50 +2023,54 @@
         <f>SUM(H3:H10)</f>
         <v>74</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="I11">
+        <f>SUM(I3:I10)</f>
+        <v>25</v>
+      </c>
+      <c r="S11" s="4">
         <v>45051</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q12" s="4">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S12" s="4">
         <v>45051</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="Q13" s="4">
+      <c r="S13" s="4">
         <v>45053</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <f>SUM(B3:J3)</f>
-        <v>54</v>
-      </c>
-      <c r="Q14" s="4">
+        <v>58</v>
+      </c>
+      <c r="S14" s="4">
         <v>45053</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2052,29 +2078,29 @@
         <f>SUM(B4:J4)</f>
         <v>42</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="S15" s="4">
         <v>45055</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B16">
         <f>SUM(B5:J5)</f>
-        <v>64</v>
-      </c>
-      <c r="Q16" s="4">
+        <v>66</v>
+      </c>
+      <c r="S16" s="4">
         <v>45058</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2082,32 +2108,32 @@
         <f>SUM(B6:J6)</f>
         <v>51</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="S17" s="4">
         <v>45058</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <f>SUM(B7:I7)</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19">
         <f>SUM(B8:I8)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2116,13 +2142,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21">
         <f>SUM(B10:J10)</f>
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>15</v>
@@ -2132,13 +2158,13 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>457</v>
+        <v>482</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
@@ -2154,7 +2180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2171,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2188,7 +2214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2197,6 +2223,8 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="L25" s="2" t="s">
         <v>6</v>
       </c>
@@ -2213,7 +2241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2232,6 +2260,9 @@
       </c>
       <c r="G26" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>21</v>
@@ -2253,7 +2284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2272,8 +2303,17 @@
       <c r="F27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2295,17 +2335,30 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="H28">
+        <v>1</v>
+      </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2324,27 +2377,29 @@
       <c r="F29">
         <v>2</v>
       </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29">
+        <v>7</v>
+      </c>
+      <c r="Q29">
         <v>11</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>8</v>
+      </c>
+      <c r="S29">
+        <v>13</v>
+      </c>
+      <c r="T29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2371,81 +2426,62 @@
         <f>SUM(G27:G29)</f>
         <v>1</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K30">
+      <c r="H30">
+        <f>SUM(H27:H29)</f>
+        <v>1</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ref="O31:T31" si="1">SUM(O29:O30)</f>
         <v>2</v>
       </c>
-      <c r="L30">
-        <v>7</v>
-      </c>
-      <c r="M30">
-        <v>11</v>
-      </c>
-      <c r="N30">
-        <v>8</v>
-      </c>
-      <c r="O30">
-        <v>13</v>
-      </c>
-      <c r="P30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
       <c r="P31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32">
-        <f t="shared" ref="K32:P32" si="1">SUM(K30:K31)</f>
-        <v>2</v>
-      </c>
-      <c r="L32">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="M32">
+      <c r="Q31">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="N32">
+      <c r="R31">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O32">
+      <c r="S31">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="P32">
+      <c r="T31">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2455,8 +2491,19 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="N33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2479,17 +2526,33 @@
       <c r="H34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2514,30 +2577,35 @@
       <c r="H35">
         <v>4</v>
       </c>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>5</v>
+      </c>
+      <c r="Q35">
+        <v>5</v>
+      </c>
+      <c r="R35">
+        <v>4</v>
+      </c>
+      <c r="S35">
+        <v>4</v>
+      </c>
+      <c r="T35">
+        <v>3</v>
+      </c>
+      <c r="U35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2562,32 +2630,35 @@
       <c r="H36">
         <v>6</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="I36">
         <v>4</v>
       </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
+      <c r="N36" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="M36">
-        <v>5</v>
-      </c>
-      <c r="N36">
-        <v>4</v>
       </c>
       <c r="O36">
         <v>4</v>
       </c>
       <c r="P36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q36">
+        <v>5</v>
+      </c>
+      <c r="R36">
+        <v>8</v>
+      </c>
+      <c r="S36">
+        <v>2</v>
+      </c>
+      <c r="T36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2612,32 +2683,40 @@
       <c r="H37">
         <v>4</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K37">
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O37">
+        <f>SUM(O35:O36)</f>
         <v>4</v>
       </c>
-      <c r="L37">
+      <c r="P37">
+        <f>SUM(P35:P36)</f>
+        <v>9</v>
+      </c>
+      <c r="Q37">
+        <f>SUM(Q35:Q36)</f>
+        <v>10</v>
+      </c>
+      <c r="R37">
+        <f>SUM(R35:R36)</f>
+        <v>12</v>
+      </c>
+      <c r="S37">
+        <v>6</v>
+      </c>
+      <c r="T37">
+        <f>SUM(T35:T36)</f>
+        <v>7</v>
+      </c>
+      <c r="U37">
         <v>4</v>
       </c>
-      <c r="M37">
-        <v>5</v>
-      </c>
-      <c r="N37">
-        <v>8</v>
-      </c>
-      <c r="O37">
-        <v>2</v>
-      </c>
-      <c r="P37">
-        <v>4</v>
-      </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2668,53 +2747,52 @@
         <f>SUM(H35:H37)</f>
         <v>14</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K38">
-        <f>SUM(K36:K37)</f>
-        <v>4</v>
-      </c>
-      <c r="L38">
-        <f>SUM(L36:L37)</f>
-        <v>9</v>
-      </c>
-      <c r="M38">
-        <f>SUM(M36:M37)</f>
-        <v>10</v>
-      </c>
-      <c r="N38">
-        <f>SUM(N36:N37)</f>
-        <v>12</v>
-      </c>
-      <c r="O38">
-        <v>6</v>
-      </c>
-      <c r="P38">
-        <f>SUM(P36:P37)</f>
-        <v>7</v>
-      </c>
-      <c r="Q38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f>SUM(I35:I37)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="E41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2722,30 +2800,32 @@
         <f>SUM(M26:P26)</f>
         <v>43</v>
       </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>2</v>
+      </c>
+      <c r="P42">
+        <v>3</v>
+      </c>
+      <c r="Q42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2753,168 +2833,144 @@
         <f>SUM(B30:F30)</f>
         <v>44</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="J43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43">
         <v>5</v>
       </c>
-      <c r="F43">
-        <v>2</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>2</v>
-      </c>
-      <c r="K43">
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
         <v>3</v>
       </c>
-      <c r="L43">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
       <c r="B44">
-        <f>SUM(F47:K47)</f>
+        <f>SUM(K46:P46)</f>
         <v>24</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44">
-        <v>5</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
+      <c r="J44" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="K44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L44">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(K38:P38)</f>
+        <f>SUM(O37:T37)</f>
         <v>48</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45">
-        <v>4</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
+      <c r="J45" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>2</v>
+      </c>
+      <c r="P45">
+        <v>2</v>
+      </c>
+      <c r="Q45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(K32:P32)</f>
+        <f>SUM(O31:T31)</f>
         <v>49</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <v>2</v>
+      <c r="J46" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="K46">
-        <v>2</v>
+        <f t="shared" ref="K46:P46" si="2">SUM(K42:K45)</f>
+        <v>11</v>
       </c>
       <c r="L46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Q46">
+        <f>SUM(Q42:Q45)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
       <c r="B47">
         <f>SUM(B38:G38)</f>
         <v>36</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F47">
-        <f t="shared" ref="F47:K47" si="2">SUM(F43:F46)</f>
-        <v>11</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="L47">
-        <f>SUM(L43:L46)</f>
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added blog 9 and updated timesheet -Quite a few blogs missing this week so timesheet not very impressive
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E355F4-A051-4832-9146-CDF5EB810641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2186142-7B30-4790-8B12-874B322BDCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
   <si>
     <t>Week 1</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Time Spent on Integration</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Integ</t>
   </si>
 </sst>
 </file>
@@ -651,13 +663,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>51</c:v>
@@ -1334,14 +1346,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1666,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
-  <dimension ref="A1:U47"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,6 +1702,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1717,6 +1730,9 @@
       <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="S2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1751,6 +1767,9 @@
       <c r="I3">
         <v>4</v>
       </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -1780,6 +1799,12 @@
       <c r="H4">
         <v>9</v>
       </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
       <c r="S4" t="s">
         <v>35</v>
       </c>
@@ -1815,6 +1840,9 @@
       <c r="I5">
         <v>2</v>
       </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
       <c r="S5" s="4">
         <v>45032</v>
       </c>
@@ -2025,7 +2053,11 @@
       </c>
       <c r="I11">
         <f>SUM(I3:I10)</f>
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="J11">
+        <f>SUM(J3:J10)</f>
+        <v>22</v>
       </c>
       <c r="S11" s="4">
         <v>45051</v>
@@ -2061,7 +2093,7 @@
       </c>
       <c r="B14">
         <f>SUM(B3:J3)</f>
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="S14" s="4">
         <v>45053</v>
@@ -2076,7 +2108,7 @@
       </c>
       <c r="B15">
         <f>SUM(B4:J4)</f>
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="S15" s="4">
         <v>45055</v>
@@ -2091,7 +2123,7 @@
       </c>
       <c r="B16">
         <f>SUM(B5:J5)</f>
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="S16" s="4">
         <v>45058</v>
@@ -2100,7 +2132,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2108,6 +2140,19 @@
         <f>SUM(B6:J6)</f>
         <v>51</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
       <c r="S17" s="4">
         <v>45058</v>
       </c>
@@ -2115,25 +2160,75 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18">
-        <f>SUM(B7:I7)</f>
+        <f>SUM(B7:J7)</f>
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19">
-        <f>SUM(B8:I8)</f>
+        <f>SUM(B8:J8)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>7</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2141,8 +2236,26 @@
         <f>SUM(B9:J9)</f>
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2150,71 +2263,104 @@
         <f>SUM(B10:J10)</f>
         <v>79</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>482</v>
+        <v>508</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <f>SUM(F19:F21)</f>
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <f>SUM(G19:G21)</f>
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <f>SUM(H19:H21)</f>
+        <v>19</v>
+      </c>
+      <c r="I22">
+        <f>SUM(I19:I21)</f>
+        <v>12</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1" t="s">
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L23" s="2" t="s">
+      <c r="P23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>7</v>
+      </c>
+      <c r="N24">
+        <v>11</v>
+      </c>
+      <c r="O24">
         <v>8</v>
       </c>
-      <c r="M23">
-        <v>3</v>
-      </c>
-      <c r="N23">
+      <c r="P24">
+        <v>13</v>
+      </c>
+      <c r="Q24">
         <v>2</v>
       </c>
-      <c r="O23">
-        <v>4</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M24">
-        <v>3</v>
-      </c>
-      <c r="N24">
-        <v>4</v>
-      </c>
-      <c r="O24">
-        <v>12</v>
-      </c>
-      <c r="P24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2225,9 +2371,12 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="L25" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
       <c r="M25">
         <v>0</v>
       </c>
@@ -2235,13 +2384,16 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2264,27 +2416,35 @@
       <c r="H26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L26">
+        <f t="shared" ref="L26:Q26" si="1">SUM(L24:L25)</f>
+        <v>2</v>
+      </c>
       <c r="M26">
-        <f>SUM(M23:M25)</f>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="N26">
-        <f>SUM(N23:N25)</f>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="O26">
-        <f>SUM(O23:O25)</f>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="P26">
-        <f>SUM(P23:P25)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2303,17 +2463,8 @@
       <c r="F27">
         <v>4</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2338,27 +2489,17 @@
       <c r="H28">
         <v>1</v>
       </c>
+      <c r="L28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2377,29 +2518,36 @@
       <c r="F29">
         <v>2</v>
       </c>
-      <c r="N29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O29">
-        <v>2</v>
-      </c>
-      <c r="P29">
-        <v>7</v>
-      </c>
-      <c r="Q29">
+      <c r="L29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R29">
-        <v>8</v>
-      </c>
-      <c r="S29">
-        <v>13</v>
-      </c>
-      <c r="T29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2430,58 +2578,99 @@
         <f>SUM(H27:H29)</f>
         <v>1</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="L30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>5</v>
+      </c>
+      <c r="O30">
+        <v>5</v>
+      </c>
+      <c r="P30">
+        <v>4</v>
+      </c>
+      <c r="Q30">
+        <v>4</v>
+      </c>
+      <c r="R30">
+        <v>3</v>
+      </c>
+      <c r="S30">
+        <v>4</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M31">
+        <v>4</v>
+      </c>
+      <c r="N31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="P31">
+        <v>8</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="R31">
+        <v>4</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32">
+        <f>SUM(M30:M31)</f>
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <f>SUM(N30:N31)</f>
+        <v>9</v>
+      </c>
+      <c r="O32">
+        <f>SUM(O30:O31)</f>
+        <v>10</v>
+      </c>
+      <c r="P32">
+        <f>SUM(P30:P31)</f>
+        <v>12</v>
+      </c>
+      <c r="Q32">
         <v>6</v>
       </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-      <c r="T30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31">
-        <f t="shared" ref="O31:T31" si="1">SUM(O29:O30)</f>
-        <v>2</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="1"/>
+      <c r="R32">
+        <f>SUM(R30:R31)</f>
         <v>7</v>
       </c>
-      <c r="Q31">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>4</v>
+      </c>
+      <c r="T32">
+        <f>SUM(T30:T31)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2493,17 +2682,8 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="N33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2529,30 +2709,11 @@
       <c r="I34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J34" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2580,32 +2741,11 @@
       <c r="I35">
         <v>2</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="J35">
         <v>4</v>
       </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>5</v>
-      </c>
-      <c r="Q35">
-        <v>5</v>
-      </c>
-      <c r="R35">
-        <v>4</v>
-      </c>
-      <c r="S35">
-        <v>4</v>
-      </c>
-      <c r="T35">
-        <v>3</v>
-      </c>
-      <c r="U35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2633,32 +2773,8 @@
       <c r="I36">
         <v>4</v>
       </c>
-      <c r="N36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O36">
-        <v>4</v>
-      </c>
-      <c r="P36">
-        <v>4</v>
-      </c>
-      <c r="Q36">
-        <v>5</v>
-      </c>
-      <c r="R36">
-        <v>8</v>
-      </c>
-      <c r="S36">
-        <v>2</v>
-      </c>
-      <c r="T36">
-        <v>4</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2686,37 +2802,8 @@
       <c r="I37">
         <v>2</v>
       </c>
-      <c r="N37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O37">
-        <f>SUM(O35:O36)</f>
-        <v>4</v>
-      </c>
-      <c r="P37">
-        <f>SUM(P35:P36)</f>
-        <v>9</v>
-      </c>
-      <c r="Q37">
-        <f>SUM(Q35:Q36)</f>
-        <v>10</v>
-      </c>
-      <c r="R37">
-        <f>SUM(R35:R36)</f>
-        <v>12</v>
-      </c>
-      <c r="S37">
-        <v>6</v>
-      </c>
-      <c r="T37">
-        <f>SUM(T35:T36)</f>
-        <v>7</v>
-      </c>
-      <c r="U37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2751,226 +2838,233 @@
         <f>SUM(I35:I37)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J40" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f>SUM(J35:J37)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42">
-        <f>SUM(M26:P26)</f>
+        <f>SUM(F22:I22)</f>
         <v>43</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K42">
-        <v>2</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <v>2</v>
-      </c>
-      <c r="P42">
-        <v>3</v>
-      </c>
-      <c r="Q42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43">
-        <f>SUM(B30:F30)</f>
-        <v>44</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>9</v>
+        <f>SUM(B30:H30)</f>
+        <v>46</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
       </c>
       <c r="K43">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43">
-        <v>3</v>
-      </c>
-      <c r="Q43">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
       <c r="B44">
-        <f>SUM(K46:P46)</f>
-        <v>24</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>6</v>
+        <f>SUM(F47:L47)</f>
+        <v>47</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
       </c>
       <c r="K44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
-        <v>1</v>
-      </c>
-      <c r="P44">
-        <v>0</v>
-      </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(O37:T37)</f>
-        <v>48</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>31</v>
+        <f>SUM(M32:U32)</f>
+        <v>56</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="O45">
-        <v>2</v>
-      </c>
-      <c r="P45">
-        <v>2</v>
-      </c>
-      <c r="Q45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(O31:T31)</f>
+        <f>SUM(L26:Q26)</f>
         <v>49</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+      <c r="L46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47">
+        <f>SUM(B38:J38)</f>
+        <v>62</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K46">
-        <f t="shared" ref="K46:P46" si="2">SUM(K42:K45)</f>
+      <c r="F47">
+        <f t="shared" ref="F47:K47" si="2">SUM(F43:F46)</f>
         <v>11</v>
       </c>
-      <c r="L46">
+      <c r="G47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M46">
+      <c r="H47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N46">
+      <c r="I47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O46">
+      <c r="J47">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P46">
+      <c r="K47">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q46">
-        <f>SUM(Q42:Q45)</f>
+      <c r="L47">
+        <f>SUM(L43:L46)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B47">
-        <f>SUM(B38:G38)</f>
-        <v>36</v>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded Tyler's blog. Updated timesheet.
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2186142-7B30-4790-8B12-874B322BDCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDBE9DE-D879-4F40-9ED5-4F77BA865F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>Week 1</t>
   </si>
@@ -684,7 +684,7 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,6 +2012,9 @@
       <c r="I10">
         <v>10</v>
       </c>
+      <c r="J10">
+        <v>7</v>
+      </c>
       <c r="S10" s="4">
         <v>45048</v>
       </c>
@@ -2057,7 +2060,7 @@
       </c>
       <c r="J11">
         <f>SUM(J3:J10)</f>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="S11" s="4">
         <v>45051</v>
@@ -2092,7 +2095,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <f>SUM(B3:J3)</f>
+        <f t="shared" ref="B14:B21" si="1">SUM(B3:J3)</f>
         <v>64</v>
       </c>
       <c r="S14" s="4">
@@ -2107,7 +2110,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <f>SUM(B4:J4)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="S15" s="4">
@@ -2122,7 +2125,7 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <f>SUM(B5:J5)</f>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="S16" s="4">
@@ -2132,12 +2135,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B17">
-        <f>SUM(B6:J6)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2147,12 +2150,6 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
       <c r="S17" s="4">
         <v>45058</v>
       </c>
@@ -2160,12 +2157,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18">
-        <f>SUM(B7:J7)</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="E18" s="1"/>
@@ -2181,23 +2178,19 @@
       <c r="I18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19">
-        <f>SUM(B8:J8)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -2215,25 +2208,23 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
-        <v>4</v>
-      </c>
-      <c r="L19">
-        <v>3</v>
-      </c>
-      <c r="M19">
-        <v>7</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20">
-        <f>SUM(B9:J9)</f>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -2252,16 +2243,25 @@
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>7</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21">
-        <f>SUM(B10:J10)</f>
-        <v>79</v>
+        <f t="shared" si="1"/>
+        <v>86</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>6</v>
@@ -2278,14 +2278,26 @@
       <c r="I21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f>SUM(B14:B21)</f>
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>21</v>
@@ -2306,61 +2318,19 @@
         <f>SUM(I19:I21)</f>
         <v>12</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K23" s="1"/>
-      <c r="L23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24">
-        <v>2</v>
-      </c>
-      <c r="M24">
-        <v>7</v>
-      </c>
-      <c r="N24">
-        <v>11</v>
-      </c>
-      <c r="O24">
-        <v>8</v>
-      </c>
-      <c r="P24">
-        <v>13</v>
-      </c>
-      <c r="Q24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22">
+        <f>SUM(L20:L21)</f>
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <f>SUM(M20:M21)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2371,29 +2341,8 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="K25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2416,35 +2365,17 @@
       <c r="H26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26">
-        <f t="shared" ref="L26:Q26" si="1">SUM(L24:L25)</f>
-        <v>2</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2463,8 +2394,27 @@
       <c r="F27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K27" s="1"/>
+      <c r="L27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2489,17 +2439,29 @@
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <v>7</v>
+      </c>
+      <c r="N28">
+        <v>11</v>
+      </c>
+      <c r="O28">
+        <v>8</v>
+      </c>
+      <c r="P28">
+        <v>13</v>
+      </c>
+      <c r="Q28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2518,36 +2480,29 @@
       <c r="F29">
         <v>2</v>
       </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U29" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2578,99 +2533,35 @@
         <f>SUM(H27:H29)</f>
         <v>1</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>4</v>
+      <c r="K30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ref="L30:Q30" si="2">SUM(L28:L29)</f>
+        <v>2</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="N30">
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="O30">
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="P30">
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="Q30">
-        <v>4</v>
-      </c>
-      <c r="R30">
-        <v>3</v>
-      </c>
-      <c r="S30">
-        <v>4</v>
-      </c>
-      <c r="T30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M31">
-        <v>4</v>
-      </c>
-      <c r="N31">
-        <v>4</v>
-      </c>
-      <c r="O31">
-        <v>5</v>
-      </c>
-      <c r="P31">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q31">
-        <v>2</v>
-      </c>
-      <c r="R31">
-        <v>4</v>
-      </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32">
-        <f>SUM(M30:M31)</f>
-        <v>4</v>
-      </c>
-      <c r="N32">
-        <f>SUM(N30:N31)</f>
-        <v>9</v>
-      </c>
-      <c r="O32">
-        <f>SUM(O30:O31)</f>
-        <v>10</v>
-      </c>
-      <c r="P32">
-        <f>SUM(P30:P31)</f>
-        <v>12</v>
-      </c>
-      <c r="Q32">
-        <v>6</v>
-      </c>
-      <c r="R32">
-        <f>SUM(R30:R31)</f>
-        <v>7</v>
-      </c>
-      <c r="S32">
-        <v>4</v>
-      </c>
-      <c r="T32">
-        <f>SUM(T30:T31)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2683,7 +2574,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2712,8 +2603,17 @@
       <c r="J34" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2744,8 +2644,36 @@
       <c r="J35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2773,8 +2701,35 @@
       <c r="I36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>5</v>
+      </c>
+      <c r="O36">
+        <v>5</v>
+      </c>
+      <c r="P36">
+        <v>4</v>
+      </c>
+      <c r="Q36">
+        <v>4</v>
+      </c>
+      <c r="R36">
+        <v>3</v>
+      </c>
+      <c r="S36">
+        <v>4</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2802,8 +2757,35 @@
       <c r="I37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M37">
+        <v>4</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <v>5</v>
+      </c>
+      <c r="P37">
+        <v>8</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37">
+        <v>4</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2842,8 +2824,41 @@
         <f>SUM(J35:J37)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38">
+        <f>SUM(M36:M37)</f>
+        <v>4</v>
+      </c>
+      <c r="N38">
+        <f>SUM(N36:N37)</f>
+        <v>9</v>
+      </c>
+      <c r="O38">
+        <f>SUM(O36:O37)</f>
+        <v>10</v>
+      </c>
+      <c r="P38">
+        <f>SUM(P36:P37)</f>
+        <v>12</v>
+      </c>
+      <c r="Q38">
+        <v>6</v>
+      </c>
+      <c r="R38">
+        <f>SUM(R36:R37)</f>
+        <v>7</v>
+      </c>
+      <c r="S38">
+        <v>4</v>
+      </c>
+      <c r="T38">
+        <f>SUM(T36:T37)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2874,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2890,7 +2905,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2923,7 +2938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -2956,12 +2971,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45">
-        <f>SUM(M32:U32)</f>
+        <f>SUM(M38:U38)</f>
         <v>56</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -2989,12 +3004,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46">
-        <f>SUM(L26:Q26)</f>
+        <f>SUM(L30:Q30)</f>
         <v>49</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -3022,7 +3037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -3034,27 +3049,27 @@
         <v>21</v>
       </c>
       <c r="F47">
-        <f t="shared" ref="F47:K47" si="2">SUM(F43:F46)</f>
+        <f t="shared" ref="F47:K47" si="3">SUM(F43:F46)</f>
         <v>11</v>
       </c>
       <c r="G47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="K47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L47">
@@ -3062,7 +3077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Added title to the title screen.
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gwion\Documents\Uni work\GP9\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyrog\Documents\Uni Work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDBE9DE-D879-4F40-9ED5-4F77BA865F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0FAAEE-DD91-4693-9A42-37602CE86C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1680,17 +1680,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1704,7 +1704,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1739,7 +1739,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="S12" s="4">
         <v>45051</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -2375,7 +2375,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -2574,7 +2574,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -2613,7 +2613,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Changed character limit of names to 24, added the start of my day 2 blog, refactored comments in logic and piece package to have the updated class names for coordinate
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyrog\Documents\Uni Work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0FAAEE-DD91-4693-9A42-37602CE86C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFE5921-FA96-40F8-82B1-24C756AE2585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
@@ -1346,14 +1346,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>21907</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1681,7 +1681,7 @@
   <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Final Report to review
</commit_message>
<xml_diff>
--- a/config/GP9 time keeping.xlsx
+++ b/config/GP9 time keeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyrog\Documents\Uni Work\GP9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFE5921-FA96-40F8-82B1-24C756AE2585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B3DDFB-B082-47BA-80F4-FC4C7B45564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A6A5294-CC9B-4A3A-B2A5-F3B5E93CFA01}"/>
   </bookViews>
@@ -1680,14 +1680,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDBC723-FCEE-45B3-A579-269AA18BA770}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>